<commit_message>
Updates: National, Maseru, Mohale's Hoek
</commit_message>
<xml_diff>
--- a/ICT Coordinators.xlsx
+++ b/ICT Coordinators.xlsx
@@ -8,15 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="ICT Data Coordinators" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Masekake Lesiamo</t>
   </si>
@@ -115,6 +113,12 @@
   </si>
   <si>
     <t>Thaba-Putsoa</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Constituency</t>
   </si>
 </sst>
 </file>
@@ -449,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -463,172 +467,156 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1"/>
-      <c r="B5" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" s="1"/>
+      <c r="B6" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1"/>
-      <c r="B11" t="s">
+    <row r="12" spans="1:2">
+      <c r="A12" s="1"/>
+      <c r="B12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
         <v>20</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="1"/>
-      <c r="B14" t="s">
+    <row r="15" spans="1:2">
+      <c r="A15" s="1"/>
+      <c r="B15" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
         <v>31</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>